<commit_message>
working up seed lot proccess
</commit_message>
<xml_diff>
--- a/data/2025_SOAP_Entries.xlsx
+++ b/data/2025_SOAP_Entries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2025_winter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC1C08-292E-4747-9574-277DD1EAEA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42C4DB0-398A-441E-AD74-44BF052BC5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{9BE16891-C31A-42D5-8A43-C9EA0E6974DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9BE16891-C31A-42D5-8A43-C9EA0E6974DF}"/>
   </bookViews>
   <sheets>
     <sheet name="2025_SOAP_Entries" sheetId="1" r:id="rId1"/>
@@ -3194,7 +3194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327ACEBA-4639-4F94-8C25-D76702EB5520}">
   <dimension ref="A1:D456"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -9596,7 +9596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC2298C-93CD-4835-A500-280997B73076}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>

</xml_diff>